<commit_message>
update main table 1 (correct typo)
</commit_message>
<xml_diff>
--- a/tables/MainTable1.xlsx
+++ b/tables/MainTable1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="100">
   <si>
     <t>region</t>
   </si>
@@ -132,13 +132,16 @@
     <t>G</t>
   </si>
   <si>
-    <t>inclonclusive</t>
+    <t>inconclusive</t>
   </si>
   <si>
     <t>Xq12</t>
   </si>
   <si>
     <t>rs189618857:66156010:T:A</t>
+  </si>
+  <si>
+    <t>66156010</t>
   </si>
   <si>
     <t>Xq21.1</t>
@@ -938,8 +941,8 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5">
-        <v>66156010</v>
+      <c r="E5" t="s">
+        <v>40</v>
       </c>
       <c r="F5" t="s">
         <v>35</v>
@@ -995,10 +998,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
@@ -1060,10 +1063,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
         <v>31</v>
@@ -1125,13 +1128,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8">
         <v>100479327</v>
@@ -1182,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1190,10 +1193,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -1247,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="U9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1255,10 +1258,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
@@ -1320,10 +1323,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
         <v>31</v>
@@ -1385,10 +1388,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
         <v>31</v>
@@ -1450,10 +1453,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -1515,10 +1518,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
         <v>31</v>
@@ -1580,10 +1583,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
         <v>31</v>
@@ -1645,10 +1648,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
         <v>31</v>
@@ -1710,10 +1713,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
@@ -1778,10 +1781,10 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18">
         <v>66301811</v>
@@ -1837,19 +1840,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
         <v>66</v>
-      </c>
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" t="s">
-        <v>65</v>
       </c>
       <c r="E19">
         <v>71509443</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
         <v>35</v>
@@ -1899,19 +1902,19 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E20">
         <v>100885798</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
         <v>25</v>
@@ -1961,13 +1964,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E21">
         <v>102552032</v>
@@ -1976,7 +1979,7 @@
         <v>35</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H21">
         <v>1000000</v>
@@ -2023,13 +2026,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E22">
         <v>125602218</v>
@@ -2038,7 +2041,7 @@
         <v>35</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H22">
         <v>1000000</v>
@@ -2085,13 +2088,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E23">
         <v>133799101</v>
@@ -2100,7 +2103,7 @@
         <v>35</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H23">
         <v>1000000</v>
@@ -2147,13 +2150,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E24">
         <v>152898261</v>
@@ -2223,10 +2226,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2234,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2242,7 +2245,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2250,7 +2253,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2258,7 +2261,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2266,7 +2269,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2274,7 +2277,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2282,7 +2285,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2290,7 +2293,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2298,7 +2301,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2306,7 +2309,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2314,7 +2317,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2322,7 +2325,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2330,7 +2333,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -2338,7 +2341,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2346,7 +2349,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2354,7 +2357,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2362,7 +2365,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2370,7 +2373,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2378,7 +2381,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2386,7 +2389,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2394,7 +2397,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update main figure 1 (add kidney function as derivate of BUN association and direction)
</commit_message>
<xml_diff>
--- a/tables/MainTable1.xlsx
+++ b/tables/MainTable1.xlsx
@@ -11,15 +11,15 @@
     <sheet name="Description" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Description!$A$1:$B$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Table1!$A$1:$U$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Description!$A$1:$B$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Table1!$A$1:$V$24</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="102">
   <si>
     <t>region</t>
   </si>
@@ -78,6 +78,9 @@
     <t>CKD_assoc</t>
   </si>
   <si>
+    <t>kidneyFunction</t>
+  </si>
+  <si>
     <t>NR_indepSignals</t>
   </si>
   <si>
@@ -105,6 +108,9 @@
     <t>FALSE</t>
   </si>
   <si>
+    <t>inconclusive</t>
+  </si>
+  <si>
     <t>male driven</t>
   </si>
   <si>
@@ -117,6 +123,9 @@
     <t>eGFR_ALL</t>
   </si>
   <si>
+    <t>likely</t>
+  </si>
+  <si>
     <t>both sexes - shared</t>
   </si>
   <si>
@@ -132,18 +141,12 @@
     <t>G</t>
   </si>
   <si>
-    <t>inconclusive</t>
-  </si>
-  <si>
     <t>Xq12</t>
   </si>
   <si>
     <t>rs189618857:66156010:T:A</t>
   </si>
   <si>
-    <t>66156010</t>
-  </si>
-  <si>
     <t>Xq21.1</t>
   </si>
   <si>
@@ -313,6 +316,9 @@
   </si>
   <si>
     <t>TRUE/FALSE flag indicating nominal (one-sided) association with CKD in our data with discordant effect direction (only for eGFR)</t>
+  </si>
+  <si>
+    <t>Kidney function defined by BUN comparisin (likely: significantly associated with BUN and discordant effect direction; unlikely: significantly associated with BUN and concordant effect direction; inconclusive: not significantly associated with BUN</t>
   </si>
   <si>
     <t>Number independent signals at this loci in best setting</t>
@@ -659,7 +665,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -668,7 +674,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1">
+    <row r="1" spans="1:22" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,28 +738,31 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>8912628</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2">
         <v>1001198</v>
@@ -777,48 +786,51 @@
         <v>1.99936884629498e-07</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T2">
+        <v>27</v>
+      </c>
+      <c r="T2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2">
         <v>1</v>
       </c>
-      <c r="U2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="V2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E3">
         <v>18482665</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3">
         <v>1007739</v>
@@ -842,48 +854,51 @@
         <v>0.356637620001335</v>
       </c>
       <c r="O3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3">
+        <v>28</v>
+      </c>
+      <c r="T3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3">
         <v>1</v>
       </c>
-      <c r="U3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="V3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
         <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
       </c>
       <c r="E4">
         <v>47166532</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H4">
         <v>1000000</v>
@@ -907,48 +922,51 @@
         <v>0.593502958446173</v>
       </c>
       <c r="O4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T4">
+        <v>28</v>
+      </c>
+      <c r="T4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4">
         <v>1</v>
       </c>
-      <c r="U4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="V4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5">
+        <v>66156010</v>
+      </c>
+      <c r="F5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>1000000</v>
@@ -972,48 +990,51 @@
         <v>0.00146652245905327</v>
       </c>
       <c r="O5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T5">
+        <v>27</v>
+      </c>
+      <c r="T5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5">
         <v>1</v>
       </c>
-      <c r="U5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="V5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E6">
         <v>79925246</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H6">
         <v>1107433</v>
@@ -1037,48 +1058,51 @@
         <v>0.138729483354191</v>
       </c>
       <c r="O6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S6" t="s">
-        <v>26</v>
-      </c>
-      <c r="T6">
+        <v>27</v>
+      </c>
+      <c r="T6" t="s">
+        <v>29</v>
+      </c>
+      <c r="U6">
         <v>1</v>
       </c>
-      <c r="U6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E7">
         <v>99890204</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H7">
         <v>1000000</v>
@@ -1102,48 +1126,51 @@
         <v>0.0650583703016246</v>
       </c>
       <c r="O7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S7" t="s">
-        <v>26</v>
-      </c>
-      <c r="T7">
+        <v>27</v>
+      </c>
+      <c r="T7" t="s">
+        <v>29</v>
+      </c>
+      <c r="U7">
         <v>1</v>
       </c>
-      <c r="U7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="V7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8">
         <v>100479327</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8">
         <v>1000000</v>
@@ -1167,48 +1194,51 @@
         <v>0.000511646385060002</v>
       </c>
       <c r="O8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S8" t="s">
-        <v>26</v>
-      </c>
-      <c r="T8">
+        <v>27</v>
+      </c>
+      <c r="T8" t="s">
+        <v>29</v>
+      </c>
+      <c r="U8">
         <v>1</v>
       </c>
-      <c r="U8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+      <c r="V8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E9">
         <v>100938892</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H9">
         <v>1000000</v>
@@ -1232,48 +1262,51 @@
         <v>0.853816518819302</v>
       </c>
       <c r="O9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S9" t="s">
-        <v>26</v>
-      </c>
-      <c r="T9">
+        <v>27</v>
+      </c>
+      <c r="T9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9">
         <v>1</v>
       </c>
-      <c r="U9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="V9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E10">
         <v>102925716</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H10">
         <v>1000000</v>
@@ -1297,48 +1330,51 @@
         <v>0.25746293726927</v>
       </c>
       <c r="O10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S10" t="s">
-        <v>26</v>
-      </c>
-      <c r="T10">
+        <v>27</v>
+      </c>
+      <c r="T10" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10">
         <v>1</v>
       </c>
-      <c r="U10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="V10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E11">
         <v>106168067</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H11">
         <v>2779864</v>
@@ -1362,48 +1398,51 @@
         <v>0.810569482615086</v>
       </c>
       <c r="O11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S11" t="s">
-        <v>26</v>
-      </c>
-      <c r="T11">
+        <v>27</v>
+      </c>
+      <c r="T11" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11">
         <v>2</v>
       </c>
-      <c r="U11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="V11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E12">
         <v>109094393</v>
       </c>
       <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
         <v>25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>24</v>
       </c>
       <c r="H12">
         <v>1000000</v>
@@ -1427,48 +1466,51 @@
         <v>0.416946699758699</v>
       </c>
       <c r="O12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S12" t="s">
-        <v>26</v>
-      </c>
-      <c r="T12">
+        <v>27</v>
+      </c>
+      <c r="T12" t="s">
+        <v>29</v>
+      </c>
+      <c r="U12">
         <v>1</v>
       </c>
-      <c r="U12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+      <c r="V12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E13">
         <v>118582383</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H13">
         <v>1000000</v>
@@ -1492,48 +1534,51 @@
         <v>0.73012532497793</v>
       </c>
       <c r="O13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T13">
+        <v>27</v>
+      </c>
+      <c r="T13" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13">
         <v>1</v>
       </c>
-      <c r="U13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="V13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E14">
         <v>125656689</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H14">
         <v>1032861</v>
@@ -1557,48 +1602,51 @@
         <v>0.37909298481637</v>
       </c>
       <c r="O14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S14" t="s">
-        <v>27</v>
-      </c>
-      <c r="T14">
+        <v>28</v>
+      </c>
+      <c r="T14" t="s">
+        <v>34</v>
+      </c>
+      <c r="U14">
         <v>1</v>
       </c>
-      <c r="U14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="V14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E15">
         <v>131251326</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H15">
         <v>1570512</v>
@@ -1622,48 +1670,51 @@
         <v>0.0247921680073519</v>
       </c>
       <c r="O15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S15" t="s">
-        <v>26</v>
-      </c>
-      <c r="T15">
+        <v>27</v>
+      </c>
+      <c r="T15" t="s">
+        <v>29</v>
+      </c>
+      <c r="U15">
         <v>1</v>
       </c>
-      <c r="U15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+      <c r="V15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>133797249</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H16">
         <v>1017385</v>
@@ -1687,48 +1738,51 @@
         <v>0.0467694201228312</v>
       </c>
       <c r="O16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S16" t="s">
-        <v>27</v>
-      </c>
-      <c r="T16">
+        <v>28</v>
+      </c>
+      <c r="T16" t="s">
+        <v>34</v>
+      </c>
+      <c r="U16">
         <v>1</v>
       </c>
-      <c r="U16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
+      <c r="V16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E17">
         <v>152898260</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H17">
         <v>1005133</v>
@@ -1752,48 +1806,51 @@
         <v>0.966343856369034</v>
       </c>
       <c r="O17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S17" t="s">
-        <v>27</v>
-      </c>
-      <c r="T17">
+        <v>28</v>
+      </c>
+      <c r="T17" t="s">
+        <v>34</v>
+      </c>
+      <c r="U17">
         <v>1</v>
       </c>
-      <c r="U17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
+      <c r="V17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E18">
         <v>66301811</v>
       </c>
       <c r="F18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H18">
         <v>2351094</v>
@@ -1817,45 +1874,45 @@
         <v>0.134828948403919</v>
       </c>
       <c r="O18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R18" t="s">
-        <v>27</v>
-      </c>
-      <c r="T18">
+        <v>28</v>
+      </c>
+      <c r="U18">
         <v>1</v>
       </c>
-      <c r="U18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+      <c r="V18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
         <v>67</v>
-      </c>
-      <c r="C19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" t="s">
-        <v>66</v>
       </c>
       <c r="E19">
         <v>71509443</v>
       </c>
       <c r="F19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H19">
         <v>1000000</v>
@@ -1879,45 +1936,45 @@
         <v>0.604059808298612</v>
       </c>
       <c r="O19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R19" t="s">
-        <v>27</v>
-      </c>
-      <c r="T19">
+        <v>28</v>
+      </c>
+      <c r="U19">
         <v>1</v>
       </c>
-      <c r="U19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
+      <c r="V19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E20">
         <v>100885798</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H20">
         <v>1601201</v>
@@ -1941,45 +1998,45 @@
         <v>0.364498914882855</v>
       </c>
       <c r="O20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R20" t="s">
-        <v>26</v>
-      </c>
-      <c r="T20">
+        <v>27</v>
+      </c>
+      <c r="U20">
         <v>1</v>
       </c>
-      <c r="U20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="V20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21">
         <v>102552032</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H21">
         <v>1000000</v>
@@ -2003,45 +2060,45 @@
         <v>0.337493576560021</v>
       </c>
       <c r="O21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R21" t="s">
-        <v>27</v>
-      </c>
-      <c r="T21">
+        <v>28</v>
+      </c>
+      <c r="U21">
         <v>1</v>
       </c>
-      <c r="U21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
+      <c r="V21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22">
         <v>125602218</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H22">
         <v>1000000</v>
@@ -2065,45 +2122,45 @@
         <v>0.0343028681324493</v>
       </c>
       <c r="O22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R22" t="s">
-        <v>27</v>
-      </c>
-      <c r="T22">
+        <v>28</v>
+      </c>
+      <c r="U22">
         <v>1</v>
       </c>
-      <c r="U22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
+      <c r="V22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E23">
         <v>133799101</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H23">
         <v>1000000</v>
@@ -2127,45 +2184,45 @@
         <v>0.858061565779223</v>
       </c>
       <c r="O23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R23" t="s">
-        <v>27</v>
-      </c>
-      <c r="T23">
+        <v>28</v>
+      </c>
+      <c r="U23">
         <v>2</v>
       </c>
-      <c r="U23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="V23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E24">
         <v>152898261</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G24" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H24">
         <v>1000000</v>
@@ -2189,33 +2246,33 @@
         <v>0.145626827970106</v>
       </c>
       <c r="O24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R24" t="s">
-        <v>27</v>
-      </c>
-      <c r="T24">
+        <v>28</v>
+      </c>
+      <c r="U24">
         <v>2</v>
       </c>
-      <c r="U24" t="s">
-        <v>32</v>
+      <c r="V24" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U24"/>
+  <autoFilter ref="A1:V24"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2226,10 +2283,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2237,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2245,7 +2302,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2253,7 +2310,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2261,7 +2318,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2269,7 +2326,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2277,7 +2334,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2285,7 +2342,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2293,7 +2350,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2301,7 +2358,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2309,7 +2366,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2317,7 +2374,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2325,7 +2382,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2333,7 +2390,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -2341,7 +2398,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2349,7 +2406,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2357,7 +2414,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2365,7 +2422,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2373,7 +2430,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2381,7 +2438,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2389,7 +2446,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2397,11 +2454,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B22"/>
+  <autoFilter ref="A1:B23"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>